<commit_message>
fixed sequence files with updated constraints
</commit_message>
<xml_diff>
--- a/sequences/retrieval_blockA_fixed-middle-10_02.xlsx
+++ b/sequences/retrieval_blockA_fixed-middle-10_02.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="retrieval" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,25 +511,15 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>distance_left</t>
+          <t>img_firstTrigNumber</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>distance_right</t>
+          <t>img_secondTrigNumber</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>img_firstTrigNumber</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>img_secondTrigNumber</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>img_thirdTrigNumber</t>
         </is>
@@ -554,12 +544,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>stimuli/chair/chair_21.jpg</t>
+          <t>stimuli/dog/dog_11.jpg</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -575,19 +565,19 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N2" t="n">
         <v>1.2</v>
@@ -595,15 +585,13 @@
       <c r="O2" t="n">
         <v>0.2</v>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>5</v>
+      </c>
       <c r="R2" t="n">
-        <v>6</v>
-      </c>
-      <c r="S2" t="n">
-        <v>4</v>
-      </c>
-      <c r="T2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -626,12 +614,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>stimuli/house/house_09.jpg</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -653,15 +641,13 @@
       <c r="O3" t="n">
         <v>0.5</v>
       </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>6</v>
+      </c>
       <c r="R3" t="n">
-        <v>9</v>
-      </c>
-      <c r="S3" t="n">
-        <v>2</v>
-      </c>
-      <c r="T3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -684,42 +670,42 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>stimuli/ball/ball_16.jpg</t>
+          <t>stimuli/hammer/hammer_21.jpg</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>stimuli/chair/chair_21.jpg</t>
+          <t>stimuli/ball/ball_28.jpg</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>stimuli/chair/chair_21.jpg</t>
+          <t>stimuli/ball/ball_28.jpg</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N4" t="n">
         <v>1.5</v>
@@ -728,19 +714,13 @@
         <v>0.2</v>
       </c>
       <c r="P4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Q4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" t="n">
         <v>4</v>
-      </c>
-      <c r="T4" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -762,27 +742,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>stimuli/hammer/hammer_39.jpg</t>
+          <t>stimuli/house/house_08.jpg</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>stimuli/jacket/jacket_37.jpg</t>
+          <t>stimuli/hand/hand_28.jpg</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>stimuli/jacket/jacket_37.jpg</t>
+          <t>stimuli/hand/hand_28.jpg</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -797,7 +777,7 @@
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
         <v>1.5</v>
@@ -806,18 +786,12 @@
         <v>0.2</v>
       </c>
       <c r="P5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="Q5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R5" t="n">
-        <v>7</v>
-      </c>
-      <c r="S5" t="n">
-        <v>10</v>
-      </c>
-      <c r="T5" t="n">
         <v>6</v>
       </c>
     </row>
@@ -840,12 +814,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>stimuli/hand/hand_36.jpg</t>
+          <t>stimuli/bicycle/bicycle_33.jpg</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>stimuli/bread/bread_28.jpg</t>
+          <t>stimuli/bread/bread_26.jpg</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -881,21 +855,19 @@
       <c r="O6" t="n">
         <v>0.2</v>
       </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>3</v>
+      </c>
       <c r="R6" t="n">
-        <v>8</v>
-      </c>
-      <c r="S6" t="n">
-        <v>3</v>
-      </c>
-      <c r="T6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -912,56 +884,40 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>stimuli/bread/bread_26.jpg</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>stimuli/bread/bread_28.jpg</t>
+          <t>stimuli/hand/hand_28.jpg</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>right</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>right</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
+        <v>0.5</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>8</v>
+      </c>
       <c r="R7" t="n">
-        <v>5</v>
-      </c>
-      <c r="S7" t="n">
-        <v>3</v>
-      </c>
-      <c r="T7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -984,27 +940,27 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>stimuli/hand/hand_36.jpg</t>
+          <t>stimuli/ball/ball_28.jpg</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1019,7 +975,7 @@
       </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N8" t="n">
         <v>1.5</v>
@@ -1028,24 +984,18 @@
         <v>0.2</v>
       </c>
       <c r="P8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R8" t="n">
-        <v>8</v>
-      </c>
-      <c r="S8" t="n">
-        <v>5</v>
-      </c>
-      <c r="T8" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1062,27 +1012,23 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>stimuli/house/house_09.jpg</t>
+          <t>stimuli/dog/dog_11.jpg</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>stimuli/ball/ball_16.jpg</t>
-        </is>
-      </c>
+          <t>stimuli/house/house_08.jpg</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>stimuli/ball/ball_16.jpg</t>
+          <t>no</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1095,35 +1041,31 @@
           <t>left</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N9" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="O9" t="n">
         <v>0.2</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q9" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R9" t="n">
-        <v>9</v>
-      </c>
-      <c r="S9" t="n">
-        <v>2</v>
-      </c>
-      <c r="T9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1140,48 +1082,60 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>stimuli/hammer/hammer_39.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>stimuli/chair/chair_21.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr"/>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
       <c r="M10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="O10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+        <v>0.2</v>
+      </c>
+      <c r="P10" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>6</v>
+      </c>
       <c r="R10" t="n">
-        <v>7</v>
-      </c>
-      <c r="S10" t="n">
-        <v>4</v>
-      </c>
-      <c r="T10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1198,57 +1152,57 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>stimuli/jacket/jacket_37.jpg</t>
+          <t>stimuli/hammer/hammer_21.jpg</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>stimuli/ball/ball_16.jpg</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
+          <t>stimuli/jacket/jacket_10.jpg</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>stimuli/bicycle/bicycle_33.jpg</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>stimuli/bicycle/bicycle_33.jpg</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>left</t>
+          <t>right</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>left</t>
-        </is>
-      </c>
-      <c r="L11" t="n">
-        <v>1</v>
-      </c>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N11" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="O11" t="n">
         <v>0.2</v>
       </c>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>10</v>
+      </c>
       <c r="R11" t="n">
-        <v>10</v>
-      </c>
-      <c r="S11" t="n">
-        <v>1</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -1270,12 +1224,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>stimuli/hammer/hammer_39.jpg</t>
+          <t>stimuli/bread/bread_26.jpg</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>stimuli/chair/chair_21.jpg</t>
+          <t>stimuli/house/house_08.jpg</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -1284,12 +1238,12 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N12" t="n">
         <v>2</v>
@@ -1297,15 +1251,13 @@
       <c r="O12" t="n">
         <v>0.5</v>
       </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>9</v>
+      </c>
       <c r="R12" t="n">
-        <v>7</v>
-      </c>
-      <c r="S12" t="n">
-        <v>4</v>
-      </c>
-      <c r="T12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1328,12 +1280,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>stimuli/house/house_09.jpg</t>
+          <t>stimuli/bicycle/bicycle_33.jpg</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
+          <t>stimuli/dog/dog_11.jpg</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -1349,19 +1301,19 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>left</t>
+          <t>right</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>left</t>
+          <t>right</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
         <v>1.2</v>
@@ -1369,21 +1321,19 @@
       <c r="O13" t="n">
         <v>0.2</v>
       </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
+      <c r="P13" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>5</v>
+      </c>
       <c r="R13" t="n">
-        <v>9</v>
-      </c>
-      <c r="S13" t="n">
-        <v>2</v>
-      </c>
-      <c r="T13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1400,57 +1350,57 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>stimuli/hand/hand_36.jpg</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
+          <t>stimuli/jacket/jacket_10.jpg</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>stimuli/dog/dog_11.jpg</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>stimuli/dog/dog_11.jpg</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>right</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="O14" t="n">
         <v>0.2</v>
       </c>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>10</v>
+      </c>
       <c r="R14" t="n">
-        <v>6</v>
-      </c>
-      <c r="S14" t="n">
-        <v>8</v>
-      </c>
-      <c r="T14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -1472,27 +1422,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>stimuli/jacket/jacket_37.jpg</t>
+          <t>stimuli/hand/hand_28.jpg</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>stimuli/ball/ball_16.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>stimuli/ball/ball_16.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1507,7 +1457,7 @@
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N15" t="n">
         <v>1.5</v>
@@ -1516,24 +1466,18 @@
         <v>0.2</v>
       </c>
       <c r="P15" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="Q15" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R15" t="n">
         <v>10</v>
       </c>
-      <c r="S15" t="n">
-        <v>1</v>
-      </c>
-      <c r="T15" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1550,68 +1494,60 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>stimuli/bread/bread_28.jpg</t>
+          <t>stimuli/ball/ball_28.jpg</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>stimuli/house/house_09.jpg</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>stimuli/dog/dog_10.jpg</t>
-        </is>
-      </c>
+          <t>stimuli/hammer/hammer_21.jpg</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>stimuli/house/house_09.jpg</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>no</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>right</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr"/>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
       <c r="M16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N16" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="O16" t="n">
         <v>0.2</v>
       </c>
       <c r="P16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R16" t="n">
-        <v>3</v>
-      </c>
-      <c r="S16" t="n">
-        <v>9</v>
-      </c>
-      <c r="T16" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1628,48 +1564,62 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>stimuli/hammer/hammer_39.jpg</t>
+          <t>stimuli/hammer/hammer_21.jpg</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>stimuli/chair/chair_21.jpg</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+          <t>stimuli/chair/chair_06.jpg</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>stimuli/bread/bread_26.jpg</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>stimuli/chair/chair_06.jpg</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>stimuli/bread/bread_26.jpg</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>right</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P17" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>4</v>
+      </c>
+      <c r="R17" t="n">
         <v>3</v>
-      </c>
-      <c r="N17" t="n">
-        <v>2</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="n">
-        <v>7</v>
-      </c>
-      <c r="S17" t="n">
-        <v>4</v>
-      </c>
-      <c r="T17" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1686,68 +1636,46 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>stimuli/hand/hand_36.jpg</t>
+          <t>stimuli/bicycle/bicycle_33.jpg</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>stimuli/dog/dog_10.jpg</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>stimuli/flower/flower_02.jpg</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>stimuli/dog/dog_10.jpg</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>left</t>
-        </is>
-      </c>
+          <t>stimuli/hand/hand_28.jpg</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>left</t>
+          <t>4</t>
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N18" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="O18" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="P18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q18" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="R18" t="n">
-        <v>8</v>
-      </c>
-      <c r="S18" t="n">
-        <v>6</v>
-      </c>
-      <c r="T18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1764,63 +1692,55 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>stimuli/house/house_09.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
-        </is>
-      </c>
+          <t>stimuli/dog/dog_11.jpg</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
+          <t>no</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>right</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr"/>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N19" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="O19" t="n">
         <v>0.2</v>
       </c>
       <c r="P19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R19" t="n">
-        <v>9</v>
-      </c>
-      <c r="S19" t="n">
-        <v>5</v>
-      </c>
-      <c r="T19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1842,12 +1762,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>stimuli/ball/ball_28.jpg</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>stimuli/bread/bread_28.jpg</t>
+          <t>stimuli/house/house_08.jpg</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1875,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N20" t="n">
         <v>1.2</v>
@@ -1883,21 +1803,19 @@
       <c r="O20" t="n">
         <v>0.2</v>
       </c>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
+      <c r="P20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>9</v>
+      </c>
       <c r="R20" t="n">
-        <v>5</v>
-      </c>
-      <c r="S20" t="n">
-        <v>3</v>
-      </c>
-      <c r="T20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1914,23 +1832,27 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>stimuli/jacket/jacket_37.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>stimuli/ball/ball_16.jpg</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
+          <t>stimuli/jacket/jacket_10.jpg</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>stimuli/hammer/hammer_21.jpg</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>stimuli/hammer/hammer_21.jpg</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1943,33 +1865,29 @@
           <t>left</t>
         </is>
       </c>
-      <c r="L21" t="n">
-        <v>1</v>
-      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="O21" t="n">
         <v>0.2</v>
       </c>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
+      <c r="P21" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>10</v>
+      </c>
       <c r="R21" t="n">
-        <v>10</v>
-      </c>
-      <c r="S21" t="n">
-        <v>1</v>
-      </c>
-      <c r="T21" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1986,21 +1904,37 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
+          <t>stimuli/hammer/hammer_21.jpg</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>stimuli/bread/bread_28.jpg</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
+          <t>stimuli/chair/chair_06.jpg</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>stimuli/ball/ball_28.jpg</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>stimuli/chair/chair_06.jpg</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>stimuli/ball/ball_28.jpg</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>right</t>
         </is>
       </c>
       <c r="L22" t="inlineStr"/>
@@ -2008,26 +1942,24 @@
         <v>3</v>
       </c>
       <c r="N22" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O22" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
+        <v>0.2</v>
+      </c>
+      <c r="P22" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>4</v>
+      </c>
       <c r="R22" t="n">
-        <v>2</v>
-      </c>
-      <c r="S22" t="n">
-        <v>3</v>
-      </c>
-      <c r="T22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2044,68 +1976,60 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>stimuli/bread/bread_28.jpg</t>
-        </is>
-      </c>
+          <t>stimuli/dog/dog_11.jpg</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>stimuli/bread/bread_28.jpg</t>
+          <t>no</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>left</t>
+          <t>right</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>left</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr"/>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N23" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="O23" t="n">
         <v>0.2</v>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q23" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R23" t="n">
-        <v>6</v>
-      </c>
-      <c r="S23" t="n">
-        <v>5</v>
-      </c>
-      <c r="T23" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2122,23 +2046,27 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>stimuli/house/house_09.jpg</t>
+          <t>stimuli/bicycle/bicycle_33.jpg</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>stimuli/hand/hand_36.jpg</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>stimuli/bread/bread_26.jpg</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>stimuli/house/house_08.jpg</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>stimuli/bread/bread_26.jpg</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>stimuli/house/house_08.jpg</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2151,29 +2079,25 @@
           <t>left</t>
         </is>
       </c>
-      <c r="L24" t="n">
-        <v>1</v>
-      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N24" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="O24" t="n">
         <v>0.2</v>
       </c>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
+      <c r="P24" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>3</v>
+      </c>
       <c r="R24" t="n">
         <v>9</v>
       </c>
-      <c r="S24" t="n">
-        <v>8</v>
-      </c>
-      <c r="T24" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2194,12 +2118,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>stimuli/ball/ball_16.jpg</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>stimuli/chair/chair_21.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -2227,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N25" t="n">
         <v>1.2</v>
@@ -2235,21 +2159,19 @@
       <c r="O25" t="n">
         <v>0.2</v>
       </c>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr"/>
+      <c r="P25" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>6</v>
+      </c>
       <c r="R25" t="n">
-        <v>1</v>
-      </c>
-      <c r="S25" t="n">
-        <v>4</v>
-      </c>
-      <c r="T25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2266,68 +2188,46 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>stimuli/hammer/hammer_39.jpg</t>
+          <t>stimuli/hand/hand_28.jpg</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>stimuli/jacket/jacket_37.jpg</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>stimuli/flower/flower_02.jpg</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>stimuli/jacket/jacket_37.jpg</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>right</t>
-        </is>
-      </c>
+          <t>stimuli/house/house_08.jpg</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N26" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="O26" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="P26" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q26" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R26" t="n">
-        <v>7</v>
-      </c>
-      <c r="S26" t="n">
-        <v>6</v>
-      </c>
-      <c r="T26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2344,48 +2244,60 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>stimuli/bicycle/bicycle_20.jpg</t>
+          <t>stimuli/dog/dog_11.jpg</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>stimuli/chair/chair_21.jpg</t>
+          <t>stimuli/hammer/hammer_21.jpg</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr"/>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
       <c r="M27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N27" t="n">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="O27" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr"/>
+        <v>0.2</v>
+      </c>
+      <c r="P27" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>7</v>
+      </c>
       <c r="R27" t="n">
-        <v>2</v>
-      </c>
-      <c r="S27" t="n">
-        <v>4</v>
-      </c>
-      <c r="T27" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2402,23 +2314,27 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>stimuli/hand/hand_36.jpg</t>
+          <t>stimuli/chair/chair_06.jpg</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>stimuli/hammer/hammer_39.jpg</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
+          <t>stimuli/hammer/hammer_21.jpg</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>stimuli/ball/ball_28.jpg</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>stimuli/hammer/hammer_21.jpg</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>stimuli/ball/ball_28.jpg</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2431,28 +2347,24 @@
           <t>right</t>
         </is>
       </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
+      <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N28" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="O28" t="n">
         <v>0.2</v>
       </c>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
+      <c r="P28" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>7</v>
+      </c>
       <c r="R28" t="n">
-        <v>8</v>
-      </c>
-      <c r="S28" t="n">
-        <v>7</v>
-      </c>
-      <c r="T28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -2474,12 +2386,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>stimuli/ball/ball_16.jpg</t>
+          <t>stimuli/flower/flower_13.jpg</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>stimuli/flower/flower_02.jpg</t>
+          <t>stimuli/bicycle/bicycle_33.jpg</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -2515,15 +2427,13 @@
       <c r="O29" t="n">
         <v>0.2</v>
       </c>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
+      <c r="P29" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>2</v>
+      </c>
       <c r="R29" t="n">
-        <v>1</v>
-      </c>
-      <c r="S29" t="n">
-        <v>6</v>
-      </c>
-      <c r="T29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2546,42 +2456,42 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>stimuli/house/house_09.jpg</t>
+          <t>stimuli/house/house_08.jpg</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>stimuli/hand/hand_28.jpg</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>stimuli/bread/bread_28.jpg</t>
+          <t>stimuli/ball/ball_28.jpg</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
+          <t>stimuli/hand/hand_28.jpg</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>stimuli/bread/bread_28.jpg</t>
+          <t>stimuli/ball/ball_28.jpg</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>right</t>
+          <t>left</t>
         </is>
       </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N30" t="n">
         <v>1.5</v>
@@ -2590,24 +2500,18 @@
         <v>0.2</v>
       </c>
       <c r="P30" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q30" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R30" t="n">
-        <v>9</v>
-      </c>
-      <c r="S30" t="n">
-        <v>5</v>
-      </c>
-      <c r="T30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2624,63 +2528,41 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>stimuli/jacket/jacket_37.jpg</t>
+          <t>stimuli/jacket/jacket_10.jpg</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>stimuli/dog/dog_10.jpg</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>stimuli/hammer/hammer_39.jpg</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>stimuli/dog/dog_10.jpg</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>stimuli/hammer/hammer_39.jpg</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>left</t>
-        </is>
-      </c>
+          <t>stimuli/bread/bread_26.jpg</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>left</t>
+          <t>5</t>
         </is>
       </c>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="n">
+        <v>4</v>
+      </c>
+      <c r="N31" t="n">
+        <v>2</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P31" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q31" t="n">
         <v>3</v>
       </c>
-      <c r="N31" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="O31" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="P31" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>4</v>
-      </c>
       <c r="R31" t="n">
-        <v>10</v>
-      </c>
-      <c r="S31" t="n">
-        <v>5</v>
-      </c>
-      <c r="T31" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>